<commit_message>
mkdir de empresa_id dentro de los subdirectorios de uploads
</commit_message>
<xml_diff>
--- a/docs/formatos/BD_Estructura.xlsx
+++ b/docs/formatos/BD_Estructura.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\formacion2.0\docs\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Flor Dominguez\Documents\Proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="USUARIOS_20150209" localSheetId="0">Hoja1!$A$7:$Q$57</definedName>
+    <definedName name="USUARIOS_20150209" localSheetId="0">Hoja1!$A$7:$N$57</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Código Empleado</t>
   </si>
@@ -69,69 +69,15 @@
     <t>Apellidos</t>
   </si>
   <si>
-    <t>Fecha ingreso a la empresa</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Correo Electrónico corporativo</t>
-  </si>
-  <si>
-    <t>Correo Electrónico personal</t>
-  </si>
-  <si>
     <t>Competencias</t>
   </si>
   <si>
-    <t>Región Geográfica</t>
-  </si>
-  <si>
     <t>País</t>
   </si>
   <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Empresa Asociada</t>
-  </si>
-  <si>
-    <t>División Funcional</t>
-  </si>
-  <si>
-    <t>Cargo</t>
-  </si>
-  <si>
-    <t>Tipo de Empleado</t>
-  </si>
-  <si>
-    <t>Valor único. No. Carnet o el generado</t>
-  </si>
-  <si>
     <t>Unico. Alfanumérico. Puede ser N.cédula, el correo, etc</t>
   </si>
   <si>
-    <t>dd/mm/aaaa</t>
-  </si>
-  <si>
-    <t>Puede ser Agencia, división del país</t>
-  </si>
-  <si>
-    <t>Ciudad de cada pais</t>
-  </si>
-  <si>
-    <t>Son las divisiones de la estructura jerárquica</t>
-  </si>
-  <si>
-    <t>Este campo permite filtrar para obtener estadísticas por tipo de empleado. Ejemplo: empleado fijo, permanente, contratado, pasante, promotor, etc</t>
-  </si>
-  <si>
-    <t>Tiene que ver con el nombre del cargo que ocupa el empleado</t>
-  </si>
-  <si>
-    <t>Tiene que ver con la estructura jeráquic. Ejemplo Vicepresidencia. Gerencias, etc.</t>
-  </si>
-  <si>
     <t>Alfabético. Sin punto. Sin comas. Se permite espacio, ñ, acentos</t>
   </si>
   <si>
@@ -141,17 +87,53 @@
     <t>Número: 0 (no ve compt) 1 (si ve comte)</t>
   </si>
   <si>
-    <t>Puede ser sub empresa dentro de la empresa</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nivel </t>
+  </si>
+  <si>
+    <t>Valor único. No. Carnet o el generado (puede ser alfa numérico)</t>
+  </si>
+  <si>
+    <t>fecha de registo</t>
+  </si>
+  <si>
+    <t>dd/mm/aaaa este será la fecha en que queda registrado el usuario en la plataforma</t>
+  </si>
+  <si>
+    <t>contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">va depender del requerimiento de la empresa y puede ser alfanumerico </t>
+  </si>
+  <si>
+    <t>Este campo se usará para el filtro de los programas, si este campo viene vacio los usuarios ven todos los programas asignados a la empresa</t>
+  </si>
+  <si>
+    <t>Correo Electrónico</t>
+  </si>
+  <si>
+    <t>campo 1</t>
+  </si>
+  <si>
+    <t>campo 2</t>
+  </si>
+  <si>
+    <t>campo 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alfanumericos y puede venir vacio </t>
+  </si>
+  <si>
+    <t>obligatorio</t>
+  </si>
+  <si>
+    <t>campo 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,19 +148,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -211,7 +193,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -229,214 +217,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>416718</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>202405</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>59532</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CuadroTexto 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4131468" y="2524125"/>
-          <a:ext cx="10429875" cy="2047876"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-VE" sz="1400"/>
-            <a:t>Los campos en rojo, son obligatorios</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-VE" sz="1400" baseline="0"/>
-            <a:t> para el sistema. Sin embargo, desde el campo 12 en adelante, no es necesario que el cliente entregue información. Puede venir en blanco o con la palabra UNICO</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-VE" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-VE" sz="1400" baseline="0"/>
-            <a:t>Los campos: 15 o 16 , se utilizan para otorgar permisos a los participantes  para ingresar a un programa en particular.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-VE" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-VE" sz="1400" baseline="0"/>
-            <a:t>La fecha de nacimiento será utilizada como contraseña; sin los puntos ni / (solo números)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-VE" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-VE" sz="1400" baseline="0"/>
-            <a:t>El correo corporativo o personal, será utilizado como Usuario/Login</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-VE" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-VE" sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>773904</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>154780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>154779</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>59530</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CuadroTexto 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3059904" y="4857749"/>
-          <a:ext cx="12406313" cy="1619250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100"/>
-            <a:t>LOS</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t> CAMPOS  12, 14, 15 DEBEN CONTENER INFORMACION DE LA ESTRUCTURA ORGANIZACIONAL DE LA EMPRESA. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>LOS CAMPOS 14 Y 15 ESTAN VINCULADOS, ES DECIR TODO CARGO DEBE ESTAR ASOCIADO A UNA DIVISIÓN FUNCIONAL, POR LO QUE PARA UNA DIVISIÓN  FUNCIONAL PUEDEN EXISTIR VARIOS CARGOS</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>LOS CAMPOS QUE VENGAN VACIOS, NOSOTROS LOS COMPLETAMOS CON UNA INFORMACIÓN ESTANDAR</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-ES" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -706,32 +486,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.7109375" customWidth="1"/>
-    <col min="17" max="17" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -740,7 +519,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2">
-        <f t="shared" ref="C1:Q1" si="0">1+B1</f>
+        <f t="shared" ref="C1:G1" si="0">1+B1</f>
         <v>3</v>
       </c>
       <c r="D1" s="2">
@@ -760,47 +539,35 @@
         <v>7</v>
       </c>
       <c r="H1" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H1" si="1">1+G1</f>
         <v>8</v>
       </c>
       <c r="I1" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I1" si="2">1+H1</f>
         <v>9</v>
       </c>
       <c r="J1" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J1" si="3">1+I1</f>
         <v>10</v>
       </c>
       <c r="K1" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K1" si="4">1+J1</f>
         <v>11</v>
       </c>
       <c r="L1" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L1" si="5">1+K1</f>
         <v>12</v>
       </c>
       <c r="M1" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M1" si="6">1+L1</f>
         <v>13</v>
       </c>
       <c r="N1" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N1" si="7">1+M1</f>
         <v>14</v>
       </c>
-      <c r="O1" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="P1" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="Q1" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -814,154 +581,138 @@
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="J2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="3" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:17" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:17" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
@@ -1132,6 +883,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>